<commit_message>
show events for self
</commit_message>
<xml_diff>
--- a/~bus dev/Penn Community.xlsx
+++ b/~bus dev/Penn Community.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="7580" yWindow="0" windowWidth="21220" windowHeight="15560" tabRatio="500"/>
@@ -130,9 +130,6 @@
     <t>https://www.law.upenn.edu/academics/crossdisciplinary/jdmba/contact.php</t>
   </si>
   <si>
-    <t>Lois MacNamara</t>
-  </si>
-  <si>
     <t>http://www.gse.upenn.edu/students/welcome</t>
   </si>
   <si>
@@ -359,6 +356,9 @@
   </si>
   <si>
     <t>Apply for funding</t>
+  </si>
+  <si>
+    <t>Lois McNamara</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1043,25 +1043,25 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>33</v>
@@ -1078,10 +1078,10 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>25</v>
@@ -1095,13 +1095,13 @@
         <v>2193</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>2</v>
@@ -1115,16 +1115,16 @@
         <v>1783</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1138,16 +1138,16 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>5</v>
@@ -1164,10 +1164,10 @@
         <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>6</v>
@@ -1184,13 +1184,13 @@
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>35</v>
@@ -1210,16 +1210,16 @@
         <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1233,13 +1233,13 @@
         <v>12</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>10</v>
@@ -1256,16 +1256,16 @@
         <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1279,13 +1279,13 @@
         <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>19</v>
@@ -1302,13 +1302,13 @@
         <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>17</v>
@@ -1316,13 +1316,13 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
         <v>81</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1353,13 +1353,13 @@
         <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1404,56 +1404,56 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="5"/>
       <c r="E23" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="5"/>
       <c r="E24" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="5"/>
       <c r="E25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="5"/>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1467,7 +1467,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1475,7 +1475,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1483,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1491,7 +1491,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1499,7 +1499,7 @@
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1515,7 +1515,7 @@
         <v>13</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1523,7 +1523,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1531,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1539,7 +1539,7 @@
         <v>20</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1547,7 +1547,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1577,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -1595,47 +1595,47 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="I2" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
         <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -1660,10 +1660,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -1688,10 +1688,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -1716,10 +1716,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -1762,21 +1762,21 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
         <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1795,10 +1795,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1806,10 +1806,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <v>2</v>

</xml_diff>